<commit_message>
corrected grid unit conversion factor
</commit_message>
<xml_diff>
--- a/examples/toy example/data/lca/unit_conversion.xlsx
+++ b/examples/toy example/data/lca/unit_conversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\mescal\examples\toy example\data\lca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777D4BF6-21CD-4D87-BCAA-8240C68FBCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E4B9E3-375F-4143-84D4-80DAB3BDCA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{98EEC620-80BF-4D8C-B6B6-060EA45EA15E}"/>
   </bookViews>
@@ -152,9 +152,6 @@
     <t>3900 GJ/kg (World Nuclear Association)</t>
   </si>
   <si>
-    <t>25000 km of lines on Tatooine (own estimations)</t>
-  </si>
-  <si>
     <t>hard coal</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>Nuclear fuel heat value: 3900 GJ/kg (World Nuclear Association)</t>
+  </si>
+  <si>
+    <t>Typical power size connected to the high-voltage electricity grid: P_HV = 500 MW, mean high-voltage electricity grid transportation length: l_HV = 11.5 km (Schnidrig et al., 2023)</t>
   </si>
 </sst>
 </file>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEFC4C7-3F00-4804-88C2-92C3F187168A}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -915,16 +915,17 @@
         <v>7</v>
       </c>
       <c r="C19" s="1">
-        <v>25000</v>
+        <f>11.5/0.5 / 1000000</f>
+        <v>2.3E-5</v>
       </c>
       <c r="D19" t="s">
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -992,10 +993,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
         <v>39</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
       </c>
       <c r="C23">
         <f>1/(9.06*0.95)</f>
@@ -1008,15 +1009,15 @@
         <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24">
         <f>1 / (13.1*0.777)</f>
@@ -1029,15 +1030,15 @@
         <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25">
         <f>1/(3900*1000/3.6)</f>
@@ -1050,7 +1051,7 @@
         <v>22</v>
       </c>
       <c r="F25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>